<commit_message>
better logic and add granary item
</commit_message>
<xml_diff>
--- a/Data/ExpendableItemDefine.xlsx
+++ b/Data/ExpendableItemDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13160"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1207,7 +1207,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1260,10 +1260,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>